<commit_message>
10 years Finalization data
</commit_message>
<xml_diff>
--- a/dataset/raw_bmkg/2016/Agustus-2016.xlsx
+++ b/dataset/raw_bmkg/2016/Agustus-2016.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arifi\OneDrive\Documents\skripsi\code\dataset\raw_bmkg\2016\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B4DFFB-E9B0-47B4-B2DB-26D2A4689D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Harian - Table" sheetId="1" r:id="rId4"/>
+    <sheet name="Data Harian - Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="70">
   <si>
     <t>ID WMO</t>
   </si>
@@ -230,17 +236,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -248,14 +250,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -269,63 +274,35 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="857250" cy="857250"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="" descr=""/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="0"/>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -614,33 +591,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:K40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="true" style="0"/>
-    <col min="2" max="2" width="13" customWidth="true" style="0"/>
-    <col min="3" max="3" width="13" customWidth="true" style="0"/>
-    <col min="4" max="4" width="13" customWidth="true" style="0"/>
-    <col min="5" max="5" width="13" customWidth="true" style="0"/>
-    <col min="6" max="6" width="13" customWidth="true" style="0"/>
-    <col min="7" max="7" width="13" customWidth="true" style="0"/>
-    <col min="8" max="8" width="13" customWidth="true" style="0"/>
-    <col min="9" max="9" width="13" customWidth="true" style="0"/>
-    <col min="10" max="10" width="13" customWidth="true" style="0"/>
-    <col min="11" max="11" width="13" customWidth="true" style="0"/>
+    <col min="1" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -648,7 +611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -656,7 +619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -664,7 +627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -672,7 +635,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -680,7 +643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -715,7 +678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -750,7 +713,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -785,7 +748,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -820,7 +783,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
@@ -838,7 +801,7 @@
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H13" s="2">
         <v>7</v>
@@ -853,7 +816,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
@@ -888,7 +851,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
@@ -923,7 +886,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -931,7 +894,7 @@
         <v>25.9</v>
       </c>
       <c r="C16" s="2">
-        <v>32.8</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="D16" s="2">
         <v>29.2</v>
@@ -943,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="2">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H16" s="2">
         <v>7</v>
@@ -958,7 +921,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
@@ -993,7 +956,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -1028,7 +991,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -1063,7 +1026,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1096,7 +1059,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1129,7 +1092,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
@@ -1137,7 +1100,7 @@
         <v>26.2</v>
       </c>
       <c r="C22" s="2">
-        <v>32.8</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="D22" s="2">
         <v>29.1</v>
@@ -1164,7 +1127,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
@@ -1199,7 +1162,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>39</v>
       </c>
@@ -1207,7 +1170,7 @@
         <v>26</v>
       </c>
       <c r="C24" s="2">
-        <v>32.8</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="D24" s="2">
         <v>29</v>
@@ -1234,7 +1197,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
@@ -1242,7 +1205,7 @@
         <v>25.5</v>
       </c>
       <c r="C25" s="2">
-        <v>32.7</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="D25" s="2">
         <v>29.8</v>
@@ -1269,7 +1232,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>41</v>
       </c>
@@ -1289,7 +1252,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="2">
-        <v>9.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="H26" s="2">
         <v>8</v>
@@ -1304,7 +1267,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>42</v>
       </c>
@@ -1337,7 +1300,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>43</v>
       </c>
@@ -1372,7 +1335,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>44</v>
       </c>
@@ -1380,7 +1343,7 @@
         <v>23.6</v>
       </c>
       <c r="C29" s="2">
-        <v>32.2</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="D29" s="2">
         <v>29.3</v>
@@ -1407,7 +1370,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>45</v>
       </c>
@@ -1427,7 +1390,7 @@
         <v>8888</v>
       </c>
       <c r="G30" s="2">
-        <v>8.8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="H30" s="2">
         <v>8</v>
@@ -1442,7 +1405,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>46</v>
       </c>
@@ -1462,7 +1425,7 @@
         <v>21.7</v>
       </c>
       <c r="G31" s="2">
-        <v>8.8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="H31" s="2">
         <v>6</v>
@@ -1477,7 +1440,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>48</v>
       </c>
@@ -1485,7 +1448,7 @@
         <v>26.2</v>
       </c>
       <c r="C32" s="2">
-        <v>32.8</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="D32" s="2">
         <v>28.7</v>
@@ -1512,7 +1475,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>49</v>
       </c>
@@ -1547,7 +1510,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>50</v>
       </c>
@@ -1564,7 +1527,7 @@
         <v>81</v>
       </c>
       <c r="F34" s="2">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G34" s="2">
         <v>1.6</v>
@@ -1582,7 +1545,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
@@ -1602,7 +1565,7 @@
         <v>7.5</v>
       </c>
       <c r="G35" s="2">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H35" s="2">
         <v>6</v>
@@ -1617,7 +1580,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>52</v>
       </c>
@@ -1652,7 +1615,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>53</v>
       </c>
@@ -1685,7 +1648,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>54</v>
       </c>
@@ -1718,7 +1681,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>55</v>
       </c>
@@ -1738,7 +1701,7 @@
         <v>3.3</v>
       </c>
       <c r="G39" s="2">
-        <v>9.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="H39" s="2">
         <v>4</v>
@@ -1753,7 +1716,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>56</v>
       </c>
@@ -1788,84 +1751,1197 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B332380C-4FD4-4F3E-94BC-50EF0BD500D4}">
+  <dimension ref="A1:K32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2">
+        <v>29.9</v>
+      </c>
+      <c r="D2" s="2">
+        <v>26.9</v>
+      </c>
+      <c r="E2" s="2">
+        <v>86</v>
+      </c>
+      <c r="F2" s="2">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5.9</v>
+      </c>
+      <c r="H2" s="2">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2">
+        <v>280</v>
+      </c>
+      <c r="J2" s="2">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2">
+        <v>25.4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2">
+        <v>28.5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>78</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="H3" s="2">
+        <v>9</v>
+      </c>
+      <c r="I3" s="2">
+        <v>290</v>
+      </c>
+      <c r="J3" s="2">
+        <v>3</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2">
+        <v>29.7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>26.4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>88</v>
+      </c>
+      <c r="F4" s="2">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2">
+        <v>7.4</v>
+      </c>
+      <c r="H4" s="2">
+        <v>4</v>
+      </c>
+      <c r="I4" s="2">
+        <v>220</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2">
+        <v>22.8</v>
+      </c>
+      <c r="C5" s="2">
+        <v>30.8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2">
+        <v>78</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H5" s="2">
+        <v>7</v>
+      </c>
+      <c r="I5" s="2">
+        <v>200</v>
+      </c>
+      <c r="J5" s="2">
+        <v>3</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2">
+        <v>26.2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>32.4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>28.8</v>
+      </c>
+      <c r="E6" s="2">
+        <v>81</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>6.3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>15</v>
+      </c>
+      <c r="I6" s="2">
+        <v>150</v>
+      </c>
+      <c r="J6" s="2">
+        <v>3</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2">
+        <v>25.8</v>
+      </c>
+      <c r="C7" s="2">
+        <v>33</v>
+      </c>
+      <c r="D7" s="2">
+        <v>28.6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>81</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>5</v>
+      </c>
+      <c r="H7" s="2">
+        <v>6</v>
+      </c>
+      <c r="I7" s="2">
+        <v>180</v>
+      </c>
+      <c r="J7" s="2">
+        <v>3</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2">
+        <v>25.9</v>
+      </c>
+      <c r="C8" s="2">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="D8" s="2">
+        <v>29.2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>80</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H8" s="2">
+        <v>7</v>
+      </c>
+      <c r="I8" s="2">
+        <v>200</v>
+      </c>
+      <c r="J8" s="2">
+        <v>3</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2">
+        <v>26.8</v>
+      </c>
+      <c r="C9" s="2">
+        <v>32.1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>29</v>
+      </c>
+      <c r="E9" s="2">
+        <v>83</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>7.7</v>
+      </c>
+      <c r="H9" s="2">
+        <v>6</v>
+      </c>
+      <c r="I9" s="2">
+        <v>150</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2">
+        <v>31.6</v>
+      </c>
+      <c r="D10" s="2">
+        <v>28</v>
+      </c>
+      <c r="E10" s="2">
+        <v>80</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="H10" s="2">
+        <v>6</v>
+      </c>
+      <c r="I10" s="2">
+        <v>190</v>
+      </c>
+      <c r="J10" s="2">
+        <v>3</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2">
+        <v>25.8</v>
+      </c>
+      <c r="C11" s="2">
+        <v>33.4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>29.4</v>
+      </c>
+      <c r="E11" s="2">
+        <v>80</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>6</v>
+      </c>
+      <c r="I11" s="2">
+        <v>190</v>
+      </c>
+      <c r="J11" s="2">
+        <v>3</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="2">
+        <v>26.2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>28.8</v>
+      </c>
+      <c r="E12" s="2">
+        <v>77</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2">
+        <v>8.4</v>
+      </c>
+      <c r="H12" s="2">
+        <v>9</v>
+      </c>
+      <c r="I12" s="2">
+        <v>180</v>
+      </c>
+      <c r="J12" s="2">
+        <v>3</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2">
+        <v>26.4</v>
+      </c>
+      <c r="C13" s="2">
+        <v>32.6</v>
+      </c>
+      <c r="D13" s="2">
+        <v>28.6</v>
+      </c>
+      <c r="E13" s="2">
+        <v>80</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2">
+        <v>6.8</v>
+      </c>
+      <c r="H13" s="2">
+        <v>7</v>
+      </c>
+      <c r="I13" s="2">
+        <v>190</v>
+      </c>
+      <c r="J13" s="2">
+        <v>3</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="2">
+        <v>26.2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="D14" s="2">
+        <v>29.1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>76</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5.7</v>
+      </c>
+      <c r="H14" s="2">
+        <v>8</v>
+      </c>
+      <c r="I14" s="2">
+        <v>230</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2">
+        <v>26.4</v>
+      </c>
+      <c r="C15" s="2">
+        <v>30.8</v>
+      </c>
+      <c r="D15" s="2">
+        <v>27.8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>81</v>
+      </c>
+      <c r="F15" s="2">
+        <v>8888</v>
+      </c>
+      <c r="G15" s="2">
+        <v>9</v>
+      </c>
+      <c r="H15" s="2">
+        <v>6</v>
+      </c>
+      <c r="I15" s="2">
+        <v>200</v>
+      </c>
+      <c r="J15" s="2">
+        <v>3</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="2">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="D16" s="2">
+        <v>29</v>
+      </c>
+      <c r="E16" s="2">
+        <v>76</v>
+      </c>
+      <c r="F16" s="2">
+        <v>8888</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2</v>
+      </c>
+      <c r="H16" s="2">
+        <v>8</v>
+      </c>
+      <c r="I16" s="2">
+        <v>190</v>
+      </c>
+      <c r="J16" s="2">
+        <v>4</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="2">
+        <v>25.5</v>
+      </c>
+      <c r="C17" s="2">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="D17" s="2">
+        <v>29.8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>77</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="H17" s="2">
+        <v>8</v>
+      </c>
+      <c r="I17" s="2">
+        <v>180</v>
+      </c>
+      <c r="J17" s="2">
+        <v>4</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="2">
+        <v>26.7</v>
+      </c>
+      <c r="C18" s="2">
+        <v>32.6</v>
+      </c>
+      <c r="D18" s="2">
+        <v>28.9</v>
+      </c>
+      <c r="E18" s="2">
+        <v>84</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="H18" s="2">
+        <v>8</v>
+      </c>
+      <c r="I18" s="2">
+        <v>160</v>
+      </c>
+      <c r="J18" s="2">
+        <v>4</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2">
+        <v>33.6</v>
+      </c>
+      <c r="D19" s="2">
+        <v>29.7</v>
+      </c>
+      <c r="E19" s="2">
+        <v>77</v>
+      </c>
+      <c r="F19" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="G19" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="H19" s="2">
+        <v>11</v>
+      </c>
+      <c r="I19" s="2">
+        <v>240</v>
+      </c>
+      <c r="J19" s="2">
+        <v>4</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="2">
+        <v>23</v>
+      </c>
+      <c r="C20" s="2">
+        <v>30.8</v>
+      </c>
+      <c r="D20" s="2">
+        <v>27.9</v>
+      </c>
+      <c r="E20" s="2">
+        <v>83</v>
+      </c>
+      <c r="F20" s="2">
+        <v>36.6</v>
+      </c>
+      <c r="G20" s="2">
+        <v>10.9</v>
+      </c>
+      <c r="H20" s="2">
+        <v>8</v>
+      </c>
+      <c r="I20" s="2">
+        <v>190</v>
+      </c>
+      <c r="J20" s="2">
+        <v>3</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="2">
+        <v>23.6</v>
+      </c>
+      <c r="C21" s="2">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="D21" s="2">
+        <v>29.3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>77</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="G21" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="H21" s="2">
+        <v>8</v>
+      </c>
+      <c r="I21" s="2">
+        <v>180</v>
+      </c>
+      <c r="J21" s="2">
+        <v>4</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="2">
+        <v>27</v>
+      </c>
+      <c r="C22" s="2">
+        <v>29.2</v>
+      </c>
+      <c r="D22" s="2">
+        <v>26.4</v>
+      </c>
+      <c r="E22" s="2">
+        <v>92</v>
+      </c>
+      <c r="F22" s="2">
+        <v>8888</v>
+      </c>
+      <c r="G22" s="2">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="H22" s="2">
+        <v>8</v>
+      </c>
+      <c r="I22" s="2">
+        <v>320</v>
+      </c>
+      <c r="J22" s="2">
+        <v>2</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="2">
+        <v>23.2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>32</v>
+      </c>
+      <c r="D23" s="2">
+        <v>28.8</v>
+      </c>
+      <c r="E23" s="2">
+        <v>82</v>
+      </c>
+      <c r="F23" s="2">
+        <v>21.7</v>
+      </c>
+      <c r="G23" s="2">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="H23" s="2">
+        <v>6</v>
+      </c>
+      <c r="I23" s="2">
+        <v>220</v>
+      </c>
+      <c r="J23" s="2">
+        <v>2</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="2">
+        <v>26.2</v>
+      </c>
+      <c r="C24" s="2">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="D24" s="2">
+        <v>28.7</v>
+      </c>
+      <c r="E24" s="2">
+        <v>80</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="H24" s="2">
+        <v>7</v>
+      </c>
+      <c r="I24" s="2">
+        <v>180</v>
+      </c>
+      <c r="J24" s="2">
+        <v>3</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="2">
+        <v>23.2</v>
+      </c>
+      <c r="C25" s="2">
+        <v>30.6</v>
+      </c>
+      <c r="D25" s="2">
+        <v>27.6</v>
+      </c>
+      <c r="E25" s="2">
+        <v>84</v>
+      </c>
+      <c r="F25" s="2">
+        <v>20.5</v>
+      </c>
+      <c r="G25" s="2">
+        <v>10.1</v>
+      </c>
+      <c r="H25" s="2">
+        <v>6</v>
+      </c>
+      <c r="I25" s="2">
+        <v>210</v>
+      </c>
+      <c r="J25" s="2">
+        <v>3</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="2">
+        <v>24.6</v>
+      </c>
+      <c r="C26" s="2">
+        <v>32</v>
+      </c>
+      <c r="D26" s="2">
+        <v>27.5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>81</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="H26" s="2">
+        <v>7</v>
+      </c>
+      <c r="I26" s="2">
+        <v>210</v>
+      </c>
+      <c r="J26" s="2">
+        <v>4</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="2">
+        <v>24.2</v>
+      </c>
+      <c r="C27" s="2">
+        <v>32</v>
+      </c>
+      <c r="D27" s="2">
+        <v>28.7</v>
+      </c>
+      <c r="E27" s="2">
+        <v>78</v>
+      </c>
+      <c r="F27" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="G27" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H27" s="2">
+        <v>6</v>
+      </c>
+      <c r="I27" s="2">
+        <v>220</v>
+      </c>
+      <c r="J27" s="2">
+        <v>2</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="2">
+        <v>25.2</v>
+      </c>
+      <c r="C28" s="2">
+        <v>31.1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>27.7</v>
+      </c>
+      <c r="E28" s="2">
+        <v>83</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="H28" s="2">
+        <v>4</v>
+      </c>
+      <c r="I28" s="2">
+        <v>170</v>
+      </c>
+      <c r="J28" s="2">
+        <v>2</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="2">
+        <v>25.5</v>
+      </c>
+      <c r="C29" s="2">
+        <v>33</v>
+      </c>
+      <c r="D29" s="2">
+        <v>29.1</v>
+      </c>
+      <c r="E29" s="2">
+        <v>78</v>
+      </c>
+      <c r="F29" s="2">
+        <v>8888</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2">
+        <v>6</v>
+      </c>
+      <c r="I29" s="2">
+        <v>120</v>
+      </c>
+      <c r="J29" s="2">
+        <v>2</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="2">
+        <v>26.1</v>
+      </c>
+      <c r="C30" s="2">
+        <v>32.6</v>
+      </c>
+      <c r="D30" s="2">
+        <v>29.5</v>
+      </c>
+      <c r="E30" s="2">
+        <v>78</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="H30" s="2">
+        <v>7</v>
+      </c>
+      <c r="I30" s="2">
+        <v>130</v>
+      </c>
+      <c r="J30" s="2">
+        <v>3</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="2">
+        <v>26.8</v>
+      </c>
+      <c r="C31" s="2">
+        <v>29.3</v>
+      </c>
+      <c r="D31" s="2">
+        <v>25.9</v>
+      </c>
+      <c r="E31" s="2">
+        <v>93</v>
+      </c>
+      <c r="F31" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="G31" s="2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="H31" s="2">
+        <v>4</v>
+      </c>
+      <c r="I31" s="2">
+        <v>230</v>
+      </c>
+      <c r="J31" s="2">
+        <v>2</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="2">
+        <v>23.7</v>
+      </c>
+      <c r="C32" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="D32" s="2">
+        <v>27.1</v>
+      </c>
+      <c r="E32" s="2">
+        <v>87</v>
+      </c>
+      <c r="F32" s="2">
+        <v>27</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="H32" s="2">
+        <v>6</v>
+      </c>
+      <c r="I32" s="2">
+        <v>200</v>
+      </c>
+      <c r="J32" s="2">
+        <v>2</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>